<commit_message>
Create list of cruises for overview
</commit_message>
<xml_diff>
--- a/data/participants/cruises/00_List_of_iAtlantic_cruises.xlsx
+++ b/data/participants/cruises/00_List_of_iAtlantic_cruises.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sa07kb\Projects\iAtlantic\Subprojects\CO2_footprint\data\iAtlantic_cruises\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sa07kb\Projects\iAtlantic\Subprojects\CO2_footprint\data\participants\cruises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4A5B00D-ED03-43C4-90DD-4BA83DE6DDD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF84D01-D3E3-4C20-8F4E-D2B59F613D8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7440" xr2:uid="{E83CC8ED-BFAC-4DC5-B8DA-D8BEA4727C38}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="107">
   <si>
     <t>MSM75</t>
   </si>
@@ -118,6 +118,243 @@
   </si>
   <si>
     <t>June 23, 2019 - September 3, 2019</t>
+  </si>
+  <si>
+    <t>B7-2019</t>
+  </si>
+  <si>
+    <t> Bjarni Sæmundsson</t>
+  </si>
+  <si>
+    <t>June 24, 2019 - July 4, 2019</t>
+  </si>
+  <si>
+    <t>SMARTIES</t>
+  </si>
+  <si>
+    <t>July 13, 2019 - August 23, 2019</t>
+  </si>
+  <si>
+    <t>MoCha_Scan_II</t>
+  </si>
+  <si>
+    <t>July 25, 2019 - July 31, 2019</t>
+  </si>
+  <si>
+    <t>Deep Connections 2019</t>
+  </si>
+  <si>
+    <t>August 6, 2019 - September 15, 2019</t>
+  </si>
+  <si>
+    <t>NOAA Ship Okeanos Explorer</t>
+  </si>
+  <si>
+    <t>DY108/109</t>
+  </si>
+  <si>
+    <t>September 6, 2019 - October 2, 2019</t>
+  </si>
+  <si>
+    <t>SAMBA2019</t>
+  </si>
+  <si>
+    <t>FR S Algoa</t>
+  </si>
+  <si>
+    <t>October 3, 2019 - October 23, 2019</t>
+  </si>
+  <si>
+    <t>BIOIL2019</t>
+  </si>
+  <si>
+    <t>RV Alpha Crucis</t>
+  </si>
+  <si>
+    <t>November 12, 2019 - November 27, 2019</t>
+  </si>
+  <si>
+    <t>MSM88-1</t>
+  </si>
+  <si>
+    <t>November 28, 2019 - December 17, 2019</t>
+  </si>
+  <si>
+    <t>MSM88-2</t>
+  </si>
+  <si>
+    <t>December 19, 2019 - January 14, 2020</t>
+  </si>
+  <si>
+    <t>JC191</t>
+  </si>
+  <si>
+    <t> RRS James Cook</t>
+  </si>
+  <si>
+    <t>January 19, 2020 - March 1, 2020</t>
+  </si>
+  <si>
+    <t>IceAGE3</t>
+  </si>
+  <si>
+    <t>RV Sonne</t>
+  </si>
+  <si>
+    <t>June 22, 2020 - July 26, 2020</t>
+  </si>
+  <si>
+    <t>AZOMP</t>
+  </si>
+  <si>
+    <t>CCGS Hudson</t>
+  </si>
+  <si>
+    <t>June 30, 2020 - July 31, 2020</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <t>June 30, 2020 - July 30, 2020</t>
+  </si>
+  <si>
+    <t>MapGES2020</t>
+  </si>
+  <si>
+    <t>July 15, 2020 - August 15, 2020</t>
+  </si>
+  <si>
+    <t>Lula1000</t>
+  </si>
+  <si>
+    <t>Deep Walls</t>
+  </si>
+  <si>
+    <t>57N Ellett Line 2020</t>
+  </si>
+  <si>
+    <t>July 15, 2020 - August 7, 2020</t>
+  </si>
+  <si>
+    <t>MoMARSAT20</t>
+  </si>
+  <si>
+    <t>September 4, 2020 - September 30, 2020</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>September 15, 2020 - October 15, 2020</t>
+  </si>
+  <si>
+    <t>SAMBA2020</t>
+  </si>
+  <si>
+    <t>September 18, 2020 - October 3, 2020</t>
+  </si>
+  <si>
+    <t>Symons_MoM</t>
+  </si>
+  <si>
+    <t>September 22, 2020 - October 3, 2020</t>
+  </si>
+  <si>
+    <t>DY120</t>
+  </si>
+  <si>
+    <t>October 5, 2020 - October 31, 2020</t>
+  </si>
+  <si>
+    <t>MetalML – MSM96</t>
+  </si>
+  <si>
+    <t>October 10, 2020 - November 10, 2020</t>
+  </si>
+  <si>
+    <t>DY116</t>
+  </si>
+  <si>
+    <t>November 1, 2020 - November 1, 2020</t>
+  </si>
+  <si>
+    <t>TBC – USP Santos Basin 2020</t>
+  </si>
+  <si>
+    <t>November 4, 2020 - November 24, 2020</t>
+  </si>
+  <si>
+    <t>PS123</t>
+  </si>
+  <si>
+    <t> RV Polarstern</t>
+  </si>
+  <si>
+    <t>December 20, 2020 - January 30, 2021</t>
+  </si>
+  <si>
+    <t>BIOIL2020</t>
+  </si>
+  <si>
+    <t>January 1, 2021 - January 1, 2021</t>
+  </si>
+  <si>
+    <t>ChEReef</t>
+  </si>
+  <si>
+    <t>RV Thalassa</t>
+  </si>
+  <si>
+    <t>DECODE</t>
+  </si>
+  <si>
+    <t>IceDivA / SO280</t>
+  </si>
+  <si>
+    <t>January 8, 2021 - February 7, 2021</t>
+  </si>
+  <si>
+    <t>PS125</t>
+  </si>
+  <si>
+    <t>April 4, 2021 - April 29, 2021</t>
+  </si>
+  <si>
+    <t>iCorsage</t>
+  </si>
+  <si>
+    <t>April 17, 2021 - May 5, 2021</t>
+  </si>
+  <si>
+    <t>Atlantic CS4</t>
+  </si>
+  <si>
+    <t>June 1, 2021 - June 1, 2021</t>
+  </si>
+  <si>
+    <t>iMirabilis_2</t>
+  </si>
+  <si>
+    <t>RV Sarmiento de Gamboa</t>
+  </si>
+  <si>
+    <t>July 23, 2021 - September 5, 2021</t>
+  </si>
+  <si>
+    <t>iAtlantic Santos basin</t>
+  </si>
+  <si>
+    <t>October 1, 2021 - October 30, 2021</t>
+  </si>
+  <si>
+    <t>iAtlantic Vitoria-Trinidade Chain</t>
+  </si>
+  <si>
+    <t>November 4, 2021 - November 24, 2021</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -469,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DE18A7-9C53-4755-BE6D-DBDCECD6AE47}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -489,102 +726,513 @@
       <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C31" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C32" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C35" t="s">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" t="s">
+        <v>89</v>
+      </c>
+      <c r="E37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C38" t="s">
+        <v>90</v>
+      </c>
+      <c r="D38" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C39" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" t="s">
+        <v>54</v>
+      </c>
+      <c r="E39" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C40" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C42" t="s">
+        <v>97</v>
+      </c>
+      <c r="D42" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+      <c r="D43" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C44" t="s">
+        <v>102</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.35">
+      <c r="C45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45" t="s">
+        <v>44</v>
+      </c>
+      <c r="E45" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>